<commit_message>
Mark the views that we are going to work on.
</commit_message>
<xml_diff>
--- a/ref/jce_calcs.xlsx
+++ b/ref/jce_calcs.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\44563\jce5\ref\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="21810" windowHeight="11640" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="21810" windowHeight="11640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="8" r:id="rId1"/>
@@ -19,7 +24,7 @@
     <definedName name="sqft" localSheetId="3">waterproofingEstimate!$F$19</definedName>
     <definedName name="sqft">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -827,21 +832,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -850,6 +840,21 @@
     </xf>
     <xf numFmtId="43" fontId="2" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1164,7 +1169,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1178,19 +1183,19 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.375" style="47" customWidth="1"/>
-    <col min="2" max="2" width="39.125" style="45" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="47" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" style="45" customWidth="1"/>
     <col min="3" max="16384" width="9" style="47"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" ht="37.5" x14ac:dyDescent="0.3">
       <c r="B2" s="46" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" ht="75" x14ac:dyDescent="0.3">
       <c r="B4" s="45" t="s">
         <v>157</v>
       </c>
@@ -1223,32 +1228,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C58" sqref="C58:H58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.875" style="26" customWidth="1"/>
-    <col min="3" max="3" width="39.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" style="26" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.25" style="1" customWidth="1"/>
-    <col min="16" max="16" width="3.625" style="26" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.5" style="1" customWidth="1"/>
-    <col min="18" max="18" width="21.125" style="49" customWidth="1"/>
-    <col min="19" max="19" width="9.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.125" style="1"/>
+    <col min="15" max="15" width="7.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="3.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="21.140625" style="49" customWidth="1"/>
+    <col min="19" max="19" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1344,7 +1349,7 @@
       </c>
       <c r="D8" s="36">
         <f ca="1">NOW()</f>
-        <v>42670.485702546299</v>
+        <v>42676.565075925922</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1593,7 +1598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -1894,7 +1899,7 @@
       <c r="H46" s="34"/>
       <c r="I46" s="34"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>71</v>
       </c>
@@ -1921,34 +1926,34 @@
       <c r="A49" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C49" s="50" t="s">
+      <c r="C49" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="D49" s="50" t="s">
+      <c r="D49" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="E49" s="50" t="s">
+      <c r="E49" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="F49" s="50" t="s">
+      <c r="F49" s="53" t="s">
         <v>19</v>
       </c>
       <c r="G49" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="H49" s="50" t="s">
+      <c r="H49" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="I49" s="50" t="s">
+      <c r="I49" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="J49" s="50" t="s">
+      <c r="J49" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="K49" s="50" t="s">
+      <c r="K49" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="L49" s="50" t="s">
+      <c r="L49" s="53" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1956,18 +1961,18 @@
       <c r="A50" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C50" s="51"/>
-      <c r="D50" s="51"/>
-      <c r="E50" s="51"/>
-      <c r="F50" s="51"/>
+      <c r="C50" s="54"/>
+      <c r="D50" s="54"/>
+      <c r="E50" s="54"/>
+      <c r="F50" s="54"/>
       <c r="G50" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H50" s="51"/>
-      <c r="I50" s="51"/>
-      <c r="J50" s="51"/>
-      <c r="K50" s="51"/>
-      <c r="L50" s="51"/>
+      <c r="H50" s="54"/>
+      <c r="I50" s="54"/>
+      <c r="J50" s="54"/>
+      <c r="K50" s="54"/>
+      <c r="L50" s="54"/>
     </row>
     <row r="51" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
@@ -2232,15 +2237,15 @@
       <c r="H59" s="8">
         <v>100</v>
       </c>
-      <c r="I59" s="55">
+      <c r="I59" s="50">
         <f>D59*H59</f>
         <v>100</v>
       </c>
-      <c r="J59" s="56">
+      <c r="J59" s="51">
         <f>I59*$M$59</f>
         <v>54</v>
       </c>
-      <c r="K59" s="57">
+      <c r="K59" s="52">
         <f>J59/sqft</f>
         <v>1.35E-2</v>
       </c>
@@ -2278,15 +2283,15 @@
       <c r="H60" s="8">
         <v>100</v>
       </c>
-      <c r="I60" s="55">
+      <c r="I60" s="50">
         <f t="shared" ref="I60:I61" si="1">D60*H60</f>
         <v>200</v>
       </c>
-      <c r="J60" s="56">
+      <c r="J60" s="51">
         <f>I60*$M$59</f>
         <v>108</v>
       </c>
-      <c r="K60" s="57">
+      <c r="K60" s="52">
         <f>J60/sqft</f>
         <v>2.7E-2</v>
       </c>
@@ -2303,7 +2308,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>73</v>
       </c>
@@ -2325,20 +2330,20 @@
       <c r="H61" s="8">
         <v>100</v>
       </c>
-      <c r="I61" s="55">
+      <c r="I61" s="50">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="J61" s="56">
+      <c r="J61" s="51">
         <f>I61*$M$59</f>
         <v>54</v>
       </c>
-      <c r="K61" s="57">
+      <c r="K61" s="52">
         <f>J61/sqft</f>
         <v>1.35E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>73</v>
       </c>
@@ -2360,15 +2365,15 @@
       <c r="H62" s="8">
         <v>100</v>
       </c>
-      <c r="I62" s="55">
+      <c r="I62" s="50">
         <f>D62*H62</f>
         <v>200</v>
       </c>
-      <c r="J62" s="56">
+      <c r="J62" s="51">
         <f>I62*$M$59</f>
         <v>108</v>
       </c>
-      <c r="K62" s="57">
+      <c r="K62" s="52">
         <f>J62/sqft</f>
         <v>2.7E-2</v>
       </c>
@@ -2875,32 +2880,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C48" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C48" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N70" sqref="N70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.875" style="26" customWidth="1"/>
-    <col min="3" max="3" width="39.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" style="26" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.25" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5" style="1" customWidth="1"/>
-    <col min="16" max="16" width="3.625" style="26" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.5" style="1" customWidth="1"/>
-    <col min="18" max="18" width="18.875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="9.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.125" style="1"/>
+    <col min="15" max="15" width="8.42578125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="3.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="18.85546875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2996,7 +3001,7 @@
       </c>
       <c r="D8" s="36">
         <f ca="1">NOW()</f>
-        <v>42670.485702546299</v>
+        <v>42676.565075925922</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3210,10 +3215,10 @@
       <c r="C22" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="E22" s="53" t="s">
+      <c r="E22" s="55" t="s">
         <v>147</v>
       </c>
-      <c r="F22" s="54"/>
+      <c r="F22" s="56"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -3228,10 +3233,10 @@
       <c r="D23" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="E23" s="52" t="s">
+      <c r="E23" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="52"/>
+      <c r="F23" s="57"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -3240,10 +3245,10 @@
       <c r="C24" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="52" t="s">
+      <c r="E24" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="52"/>
+      <c r="F24" s="57"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -3259,7 +3264,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>145</v>
       </c>
@@ -3391,7 +3396,7 @@
       </c>
     </row>
     <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>145</v>
       </c>
@@ -3684,38 +3689,38 @@
       </c>
       <c r="C49" s="5"/>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C50" s="50" t="s">
+      <c r="C50" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="D50" s="50" t="s">
+      <c r="D50" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="E50" s="50" t="s">
+      <c r="E50" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="F50" s="50" t="s">
+      <c r="F50" s="53" t="s">
         <v>19</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="H50" s="50" t="s">
+      <c r="H50" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="I50" s="50" t="s">
+      <c r="I50" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="J50" s="50" t="s">
+      <c r="J50" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="K50" s="50" t="s">
+      <c r="K50" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="L50" s="50" t="s">
+      <c r="L50" s="53" t="s">
         <v>87</v>
       </c>
     </row>
@@ -3723,18 +3728,18 @@
       <c r="A51" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C51" s="51"/>
-      <c r="D51" s="51"/>
-      <c r="E51" s="51"/>
-      <c r="F51" s="51"/>
+      <c r="C51" s="54"/>
+      <c r="D51" s="54"/>
+      <c r="E51" s="54"/>
+      <c r="F51" s="54"/>
       <c r="G51" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H51" s="51"/>
-      <c r="I51" s="51"/>
-      <c r="J51" s="51"/>
-      <c r="K51" s="51"/>
-      <c r="L51" s="51"/>
+      <c r="H51" s="54"/>
+      <c r="I51" s="54"/>
+      <c r="J51" s="54"/>
+      <c r="K51" s="54"/>
+      <c r="L51" s="54"/>
     </row>
     <row r="52" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
@@ -4068,7 +4073,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>73</v>
       </c>
@@ -4102,7 +4107,7 @@
         <v>1.9230769230769232E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>73</v>
       </c>
@@ -4613,11 +4618,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="F50:F51"/>
     <mergeCell ref="J50:J51"/>
     <mergeCell ref="K50:K51"/>
     <mergeCell ref="L50:L51"/>
@@ -4625,6 +4625,11 @@
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="H50:H51"/>
     <mergeCell ref="I50:I51"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="F50:F51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" orientation="landscape" r:id="rId1"/>
@@ -4645,28 +4650,28 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.875" style="26" customWidth="1"/>
-    <col min="3" max="3" width="39.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" style="26" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.25" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5" style="1" customWidth="1"/>
-    <col min="16" max="16" width="8.5" style="26" customWidth="1"/>
-    <col min="17" max="17" width="8.5" style="1" customWidth="1"/>
-    <col min="18" max="18" width="17.375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="9.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.125" style="1"/>
+    <col min="15" max="15" width="8.42578125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="8.42578125" style="26" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="17.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -4762,7 +4767,7 @@
       </c>
       <c r="D8" s="36">
         <f ca="1">NOW()</f>
-        <v>42670.485702546299</v>
+        <v>42676.565075925922</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -5009,7 +5014,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>51</v>
       </c>
@@ -5173,7 +5178,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>51</v>
       </c>
@@ -5504,34 +5509,34 @@
       <c r="A50" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C50" s="50" t="s">
+      <c r="C50" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="D50" s="50" t="s">
+      <c r="D50" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="E50" s="50" t="s">
+      <c r="E50" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="F50" s="50" t="s">
+      <c r="F50" s="53" t="s">
         <v>19</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="H50" s="50" t="s">
+      <c r="H50" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="I50" s="50" t="s">
+      <c r="I50" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="J50" s="50" t="s">
+      <c r="J50" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="K50" s="50" t="s">
+      <c r="K50" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="L50" s="50" t="s">
+      <c r="L50" s="53" t="s">
         <v>87</v>
       </c>
     </row>
@@ -5539,18 +5544,18 @@
       <c r="A51" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C51" s="51"/>
-      <c r="D51" s="51"/>
-      <c r="E51" s="51"/>
-      <c r="F51" s="51"/>
+      <c r="C51" s="54"/>
+      <c r="D51" s="54"/>
+      <c r="E51" s="54"/>
+      <c r="F51" s="54"/>
       <c r="G51" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H51" s="51"/>
-      <c r="I51" s="51"/>
-      <c r="J51" s="51"/>
-      <c r="K51" s="51"/>
-      <c r="L51" s="51"/>
+      <c r="H51" s="54"/>
+      <c r="I51" s="54"/>
+      <c r="J51" s="54"/>
+      <c r="K51" s="54"/>
+      <c r="L51" s="54"/>
     </row>
     <row r="52" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
@@ -5884,7 +5889,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>73</v>
       </c>
@@ -5918,7 +5923,7 @@
         <v>2.0769230769230769E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>73</v>
       </c>

</xml_diff>